<commit_message>
Atribuição ID: 2,3,4 - Carol
</commit_message>
<xml_diff>
--- a/documento_projeto/Pixels - Relatório de Acessibilidade.xlsx
+++ b/documento_projeto/Pixels - Relatório de Acessibilidade.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carol-Gu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Fatec\pixels\documento_projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9000E924-047A-4A55-99DB-41A5F504F4D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDED8EB5-EA58-43C6-8ADE-095D314111A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Relatório" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="170">
   <si>
     <t>ID</t>
   </si>
@@ -554,7 +554,7 @@
     <numFmt numFmtId="165" formatCode="m/d/yyyy\ h:mm:ss"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -608,6 +608,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -693,7 +700,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -803,6 +810,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1022,10 +1032,10 @@
   <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N2" sqref="N2:N69"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1102,8 +1112,8 @@
       <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>16</v>
+      <c r="C2" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>17</v>
@@ -1174,7 +1184,9 @@
       <c r="M3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="N3" s="6"/>
+      <c r="N3" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="O3" s="10"/>
     </row>
     <row r="4" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1215,7 +1227,9 @@
       <c r="M4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="N4" s="6"/>
+      <c r="N4" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="O4" s="10"/>
     </row>
     <row r="5" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1256,7 +1270,9 @@
       <c r="M5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="N5" s="6"/>
+      <c r="N5" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="O5" s="10"/>
     </row>
     <row r="6" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1266,8 +1282,8 @@
       <c r="B6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>16</v>
+      <c r="C6" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>17</v>
@@ -1307,8 +1323,8 @@
       <c r="B7" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>16</v>
+      <c r="C7" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>17</v>
@@ -1348,8 +1364,8 @@
       <c r="B8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>16</v>
+      <c r="C8" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>17</v>
@@ -1389,8 +1405,8 @@
       <c r="B9" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>16</v>
+      <c r="C9" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>17</v>
@@ -1430,8 +1446,8 @@
       <c r="B10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>16</v>
+      <c r="C10" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>17</v>
@@ -1471,8 +1487,8 @@
       <c r="B11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>16</v>
+      <c r="C11" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>17</v>
@@ -1512,8 +1528,8 @@
       <c r="B12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>16</v>
+      <c r="C12" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>17</v>
@@ -1553,8 +1569,8 @@
       <c r="B13" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>16</v>
+      <c r="C13" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>17</v>
@@ -1594,8 +1610,8 @@
       <c r="B14" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>16</v>
+      <c r="C14" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>17</v>
@@ -1635,8 +1651,8 @@
       <c r="B15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>16</v>
+      <c r="C15" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>17</v>
@@ -1676,8 +1692,8 @@
       <c r="B16" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>16</v>
+      <c r="C16" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>17</v>
@@ -1717,8 +1733,8 @@
       <c r="B17" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>16</v>
+      <c r="C17" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>17</v>
@@ -1758,8 +1774,8 @@
       <c r="B18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>16</v>
+      <c r="C18" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>17</v>
@@ -1789,7 +1805,7 @@
       <c r="M18" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="N18" s="6"/>
+      <c r="N18" s="42"/>
       <c r="O18" s="10"/>
     </row>
     <row r="19" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1799,8 +1815,8 @@
       <c r="B19" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>16</v>
+      <c r="C19" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>17</v>
@@ -1840,8 +1856,8 @@
       <c r="B20" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>16</v>
+      <c r="C20" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>17</v>
@@ -1881,8 +1897,8 @@
       <c r="B21" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>16</v>
+      <c r="C21" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>17</v>
@@ -1922,8 +1938,8 @@
       <c r="B22" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>16</v>
+      <c r="C22" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>17</v>
@@ -1963,8 +1979,8 @@
       <c r="B23" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>16</v>
+      <c r="C23" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>17</v>
@@ -2004,8 +2020,8 @@
       <c r="B24" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>16</v>
+      <c r="C24" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>17</v>
@@ -2046,7 +2062,7 @@
         <v>15</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>86</v>
+        <v>134</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>87</v>
@@ -2087,7 +2103,7 @@
         <v>46</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>86</v>
+        <v>134</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>87</v>
@@ -2424,8 +2440,8 @@
       <c r="B34" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>16</v>
+      <c r="C34" s="14" t="s">
+        <v>86</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>103</v>
@@ -2506,8 +2522,8 @@
       <c r="B36" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>16</v>
+      <c r="C36" s="14" t="s">
+        <v>86</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>17</v>
@@ -2997,8 +3013,8 @@
       <c r="B49" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C49" s="5" t="s">
-        <v>16</v>
+      <c r="C49" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>17</v>
@@ -3038,8 +3054,8 @@
       <c r="B50" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C50" s="5" t="s">
-        <v>16</v>
+      <c r="C50" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>17</v>
@@ -3079,8 +3095,8 @@
       <c r="B51" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C51" s="5" t="s">
-        <v>16</v>
+      <c r="C51" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>17</v>
@@ -3120,8 +3136,8 @@
       <c r="B52" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C52" s="5" t="s">
-        <v>16</v>
+      <c r="C52" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>17</v>
@@ -3161,8 +3177,8 @@
       <c r="B53" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C53" s="5" t="s">
-        <v>16</v>
+      <c r="C53" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>17</v>
@@ -3202,8 +3218,8 @@
       <c r="B54" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>16</v>
+      <c r="C54" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>17</v>
@@ -3243,8 +3259,8 @@
       <c r="B55" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>16</v>
+      <c r="C55" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>17</v>
@@ -3284,8 +3300,8 @@
       <c r="B56" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C56" s="5" t="s">
-        <v>16</v>
+      <c r="C56" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>17</v>
@@ -3325,8 +3341,8 @@
       <c r="B57" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C57" s="5" t="s">
-        <v>16</v>
+      <c r="C57" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>17</v>
@@ -3366,8 +3382,8 @@
       <c r="B58" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C58" s="5" t="s">
-        <v>16</v>
+      <c r="C58" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>17</v>
@@ -3407,8 +3423,8 @@
       <c r="B59" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>16</v>
+      <c r="C59" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>17</v>
@@ -3448,8 +3464,8 @@
       <c r="B60" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C60" s="5" t="s">
-        <v>16</v>
+      <c r="C60" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>17</v>
@@ -3489,8 +3505,8 @@
       <c r="B61" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C61" s="5" t="s">
-        <v>16</v>
+      <c r="C61" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>17</v>
@@ -3530,8 +3546,8 @@
       <c r="B62" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C62" s="5" t="s">
-        <v>16</v>
+      <c r="C62" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>17</v>
@@ -3571,8 +3587,8 @@
       <c r="B63" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>16</v>
+      <c r="C63" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>17</v>
@@ -3612,8 +3628,8 @@
       <c r="B64" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C64" s="5" t="s">
-        <v>16</v>
+      <c r="C64" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>17</v>
@@ -3653,8 +3669,8 @@
       <c r="B65" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C65" s="5" t="s">
-        <v>16</v>
+      <c r="C65" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>17</v>
@@ -3694,8 +3710,8 @@
       <c r="B66" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C66" s="5" t="s">
-        <v>16</v>
+      <c r="C66" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>17</v>
@@ -3735,8 +3751,8 @@
       <c r="B67" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C67" s="5" t="s">
-        <v>16</v>
+      <c r="C67" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>17</v>
@@ -3776,8 +3792,8 @@
       <c r="B68" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C68" s="5" t="s">
-        <v>16</v>
+      <c r="C68" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>17</v>
@@ -3817,8 +3833,8 @@
       <c r="B69" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C69" s="5" t="s">
-        <v>16</v>
+      <c r="C69" s="14" t="s">
+        <v>134</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>17</v>
@@ -10371,7 +10387,7 @@
   </sheetData>
   <autoFilter ref="A1:O24" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10379,7 +10395,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:D1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Atualizado os textos alternativos da desnho.php
</commit_message>
<xml_diff>
--- a/documento_projeto/Pixels - Relatório de Acessibilidade.xlsx
+++ b/documento_projeto/Pixels - Relatório de Acessibilidade.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Fatec\pixels\documento_projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDED8EB5-EA58-43C6-8ADE-095D314111A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28654EFA-4EF9-41B8-81C9-567921330A54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Relatório" sheetId="1" r:id="rId1"/>
@@ -700,7 +700,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -812,6 +812,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1032,10 +1035,10 @@
   <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3:C5"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1180,7 +1183,9 @@
       <c r="K3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="L3" s="6"/>
+      <c r="L3" s="43">
+        <v>44118</v>
+      </c>
       <c r="M3" s="6" t="s">
         <v>34</v>
       </c>
@@ -1223,7 +1228,9 @@
       <c r="K4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="6"/>
+      <c r="L4" s="43">
+        <v>44112</v>
+      </c>
       <c r="M4" s="6" t="s">
         <v>34</v>
       </c>
@@ -1267,7 +1274,7 @@
         <v>42</v>
       </c>
       <c r="L5" s="6"/>
-      <c r="M5" s="6" t="s">
+      <c r="M5" s="42" t="s">
         <v>26</v>
       </c>
       <c r="N5" s="6" t="s">

</xml_diff>

<commit_message>
Atualizado os textos descritivos do quemSomos.php
</commit_message>
<xml_diff>
--- a/documento_projeto/Pixels - Relatório de Acessibilidade.xlsx
+++ b/documento_projeto/Pixels - Relatório de Acessibilidade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Fatec\pixels\documento_projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28654EFA-4EF9-41B8-81C9-567921330A54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C677BC5-B0A2-4D75-A92B-7893A0B1512A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1038,7 +1038,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1273,8 +1273,10 @@
       <c r="K5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="L5" s="6"/>
-      <c r="M5" s="42" t="s">
+      <c r="L5" s="43">
+        <v>44118</v>
+      </c>
+      <c r="M5" s="6" t="s">
         <v>26</v>
       </c>
       <c r="N5" s="6" t="s">

</xml_diff>

<commit_message>
Alterações de texto descritivo no pixelSobre.php e carreira.php
</commit_message>
<xml_diff>
--- a/documento_projeto/Pixels - Relatório de Acessibilidade.xlsx
+++ b/documento_projeto/Pixels - Relatório de Acessibilidade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Fatec\pixels\documento_projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C677BC5-B0A2-4D75-A92B-7893A0B1512A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1141F5C5-F165-428D-8BD9-449A90818EE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,14 +18,14 @@
     <sheet name="Instruções" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Relatório!$A$1:$O$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Relatório!$A$1:$O$69</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="171">
   <si>
     <t>ID</t>
   </si>
@@ -543,6 +543,9 @@
   <si>
     <t>Mapear os erros. Aqui tem duas coisas importantes: só temos UMA planilha de controle
 Não podemos ter repetição do IDs</t>
+  </si>
+  <si>
+    <t>O Talkback lê algo irreconhecível</t>
   </si>
 </sst>
 </file>
@@ -700,7 +703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -816,6 +819,12 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1035,10 +1044,10 @@
   <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N5" sqref="N5"/>
+      <selection pane="bottomRight" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1156,8 +1165,8 @@
       <c r="B3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>16</v>
+      <c r="C3" s="34" t="s">
+        <v>155</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>17</v>
@@ -1201,8 +1210,8 @@
       <c r="B4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>16</v>
+      <c r="C4" s="34" t="s">
+        <v>155</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>17</v>
@@ -1246,8 +1255,8 @@
       <c r="B5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>16</v>
+      <c r="C5" s="34" t="s">
+        <v>155</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>17</v>
@@ -1455,7 +1464,7 @@
       <c r="B10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="45" t="s">
         <v>134</v>
       </c>
       <c r="D10" s="6" t="s">
@@ -1824,8 +1833,8 @@
       <c r="B19" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>134</v>
+      <c r="C19" s="34" t="s">
+        <v>155</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>17</v>
@@ -1851,11 +1860,15 @@
       <c r="K19" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="L19" s="12"/>
+      <c r="L19" s="43">
+        <v>44118</v>
+      </c>
       <c r="M19" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="N19" s="6"/>
+      <c r="N19" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="O19" s="10"/>
     </row>
     <row r="20" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1865,8 +1878,8 @@
       <c r="B20" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>134</v>
+      <c r="C20" s="34" t="s">
+        <v>155</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>17</v>
@@ -1892,11 +1905,15 @@
       <c r="K20" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="L20" s="12"/>
+      <c r="L20" s="43">
+        <v>44118</v>
+      </c>
       <c r="M20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="N20" s="6"/>
+      <c r="N20" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="O20" s="10"/>
     </row>
     <row r="21" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1906,8 +1923,8 @@
       <c r="B21" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>134</v>
+      <c r="C21" s="34" t="s">
+        <v>155</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>17</v>
@@ -1933,11 +1950,15 @@
       <c r="K21" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="L21" s="12"/>
+      <c r="L21" s="43">
+        <v>44118</v>
+      </c>
       <c r="M21" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="N21" s="6"/>
+      <c r="N21" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="O21" s="10"/>
     </row>
     <row r="22" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3131,11 +3152,15 @@
       <c r="K51" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="L51" s="6"/>
+      <c r="L51" s="43">
+        <v>44118</v>
+      </c>
       <c r="M51" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="N51" s="6"/>
+      <c r="N51" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="O51" s="10"/>
     </row>
     <row r="52" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3719,8 +3744,8 @@
       <c r="B66" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C66" s="14" t="s">
-        <v>134</v>
+      <c r="C66" s="34" t="s">
+        <v>155</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>17</v>
@@ -3746,22 +3771,26 @@
       <c r="K66" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="L66" s="12"/>
+      <c r="L66" s="43">
+        <v>44118</v>
+      </c>
       <c r="M66" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="N66" s="6"/>
+      <c r="N66" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="O66" s="10"/>
     </row>
     <row r="67" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="6">
         <v>66</v>
       </c>
-      <c r="B67" s="9" t="s">
+      <c r="B67" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="C67" s="14" t="s">
-        <v>134</v>
+      <c r="C67" s="34" t="s">
+        <v>155</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>17</v>
@@ -3787,11 +3816,15 @@
       <c r="K67" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="L67" s="12"/>
+      <c r="L67" s="43">
+        <v>44118</v>
+      </c>
       <c r="M67" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="N67" s="6"/>
+      <c r="N67" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="O67" s="10"/>
     </row>
     <row r="68" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3858,7 +3891,7 @@
         <v>77</v>
       </c>
       <c r="H69" s="7" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="I69" s="7" t="s">
         <v>81</v>
@@ -10394,7 +10427,7 @@
       <c r="M1000" s="30"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O24" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:O69" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -10405,7 +10438,7 @@
   <dimension ref="B1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
relatorio de acessibilidade, teste de inclusão do twitter summary cards
</commit_message>
<xml_diff>
--- a/documento_projeto/Pixels - Relatório de Acessibilidade.xlsx
+++ b/documento_projeto/Pixels - Relatório de Acessibilidade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Fatec\pixels\documento_projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1141F5C5-F165-428D-8BD9-449A90818EE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D5FCBA-F8AD-42A8-A8CA-6E43328BA0A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="171">
   <si>
     <t>ID</t>
   </si>
@@ -455,9 +455,6 @@
     <t>pixel.php</t>
   </si>
   <si>
-    <t>No card "Fique por dentro", o usuario tentou acessar clicando na imagem ou titulo, mas apenas o texto era o link</t>
-  </si>
-  <si>
     <t>Ajuste da ancora</t>
   </si>
   <si>
@@ -483,9 +480,6 @@
   </si>
   <si>
     <t>Sem acesso a seta no rodapé, para retornar ao topo da página</t>
-  </si>
-  <si>
-    <t>Impossivel acessar a seta no rodapé para retornar ao topo da página, através do teclado</t>
   </si>
   <si>
     <t>impede a utilização</t>
@@ -546,6 +540,14 @@
   </si>
   <si>
     <t>O Talkback lê algo irreconhecível</t>
+  </si>
+  <si>
+    <t>No card "Fique por dentro", o usuario tentou acessar clicando na 
+imagem ou titulo, mas apenas o texto era o link</t>
+  </si>
+  <si>
+    <t>Impossivel acessar a seta no rodapé para retornar ao topo da página, 
+através do teclado</t>
   </si>
 </sst>
 </file>
@@ -557,7 +559,7 @@
     <numFmt numFmtId="165" formatCode="m/d/yyyy\ h:mm:ss"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -618,6 +620,13 @@
       <color rgb="FF000000"/>
       <name val="Cambria"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -703,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -820,12 +829,16 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1044,22 +1057,22 @@
   <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" customWidth="1"/>
     <col min="6" max="6" width="53.85546875" customWidth="1"/>
     <col min="7" max="7" width="32.42578125" customWidth="1"/>
-    <col min="8" max="8" width="55.42578125" customWidth="1"/>
+    <col min="8" max="8" width="60" customWidth="1"/>
     <col min="9" max="9" width="58.5703125" customWidth="1"/>
     <col min="10" max="10" width="11.5703125" customWidth="1"/>
     <col min="11" max="11" width="15.140625" customWidth="1"/>
@@ -1117,7 +1130,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1166,7 +1179,7 @@
         <v>27</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>17</v>
@@ -1211,7 +1224,7 @@
         <v>27</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>17</v>
@@ -1256,7 +1269,7 @@
         <v>27</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>17</v>
@@ -1300,8 +1313,8 @@
       <c r="B6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>134</v>
+      <c r="C6" s="34" t="s">
+        <v>153</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>17</v>
@@ -1327,11 +1340,15 @@
       <c r="K6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="6"/>
+      <c r="L6" s="43">
+        <v>44119</v>
+      </c>
       <c r="M6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="N6" s="6"/>
+      <c r="N6" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="O6" s="10"/>
     </row>
     <row r="7" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1464,7 +1481,7 @@
       <c r="B10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="44" t="s">
         <v>134</v>
       </c>
       <c r="D10" s="6" t="s">
@@ -1834,7 +1851,7 @@
         <v>27</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>17</v>
@@ -1879,7 +1896,7 @@
         <v>46</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>17</v>
@@ -1924,7 +1941,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>17</v>
@@ -2381,7 +2398,7 @@
       <c r="N31" s="17"/>
       <c r="O31" s="25"/>
     </row>
-    <row r="32" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -2403,7 +2420,7 @@
       <c r="G32" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="H32" s="18" t="s">
+      <c r="H32" s="45" t="s">
         <v>101</v>
       </c>
       <c r="I32" s="18" t="s">
@@ -2422,7 +2439,7 @@
       <c r="N32" s="17"/>
       <c r="O32" s="26"/>
     </row>
-    <row r="33" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -2444,7 +2461,7 @@
       <c r="G33" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="H33" s="18" t="s">
+      <c r="H33" s="45" t="s">
         <v>102</v>
       </c>
       <c r="I33" s="18" t="s">
@@ -2865,11 +2882,11 @@
       <c r="G44" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="H44" s="7" t="s">
+      <c r="H44" s="46" t="s">
+        <v>169</v>
+      </c>
+      <c r="I44" s="7" t="s">
         <v>141</v>
-      </c>
-      <c r="I44" s="7" t="s">
-        <v>142</v>
       </c>
       <c r="J44" s="6" t="s">
         <v>91</v>
@@ -2897,16 +2914,16 @@
         <v>83</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>20</v>
       </c>
       <c r="H45" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="I45" s="7" t="s">
         <v>144</v>
-      </c>
-      <c r="I45" s="7" t="s">
-        <v>145</v>
       </c>
       <c r="J45" s="27">
         <v>43840</v>
@@ -2936,16 +2953,16 @@
         <v>83</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>20</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J46" s="27">
         <v>43840</v>
@@ -2975,16 +2992,16 @@
         <v>83</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G47" s="6" t="s">
         <v>20</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J47" s="27">
         <v>43840</v>
@@ -2997,7 +3014,7 @@
       <c r="N47" s="6"/>
       <c r="O47" s="10"/>
     </row>
-    <row r="48" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <v>47</v>
       </c>
@@ -3014,16 +3031,16 @@
         <v>83</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G48" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H48" s="7" t="s">
-        <v>151</v>
+      <c r="H48" s="46" t="s">
+        <v>170</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J48" s="27">
         <v>43840</v>
@@ -3655,7 +3672,7 @@
       <c r="N63" s="6"/>
       <c r="O63" s="10"/>
     </row>
-    <row r="64" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="6">
         <v>63</v>
       </c>
@@ -3696,15 +3713,15 @@
       <c r="N64" s="6"/>
       <c r="O64" s="10"/>
     </row>
-    <row r="65" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="6">
         <v>64</v>
       </c>
       <c r="B65" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C65" s="14" t="s">
-        <v>134</v>
+      <c r="C65" s="34" t="s">
+        <v>153</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>17</v>
@@ -3730,11 +3747,15 @@
       <c r="K65" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="L65" s="12"/>
+      <c r="L65" s="43">
+        <v>44118</v>
+      </c>
       <c r="M65" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="N65" s="6"/>
+      <c r="N65" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="O65" s="10"/>
     </row>
     <row r="66" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3745,7 +3766,7 @@
         <v>46</v>
       </c>
       <c r="C66" s="34" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>17</v>
@@ -3786,11 +3807,11 @@
       <c r="A67" s="6">
         <v>66</v>
       </c>
-      <c r="B67" s="44" t="s">
+      <c r="B67" s="9" t="s">
         <v>27</v>
       </c>
       <c r="C67" s="34" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>17</v>
@@ -3891,7 +3912,7 @@
         <v>77</v>
       </c>
       <c r="H69" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="I69" s="7" t="s">
         <v>81</v>
@@ -3970,6 +3991,7 @@
       <c r="E78" s="29"/>
       <c r="F78" s="28"/>
       <c r="G78" s="29"/>
+      <c r="K78" s="47"/>
       <c r="M78" s="28"/>
     </row>
     <row r="79" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10438,7 +10460,7 @@
   <dimension ref="B1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10461,7 +10483,7 @@
       </c>
       <c r="C2" s="32"/>
       <c r="D2" s="33" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10470,7 +10492,7 @@
       </c>
       <c r="C3" s="32"/>
       <c r="D3" s="33" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10479,7 +10501,7 @@
       </c>
       <c r="C4" s="32"/>
       <c r="D4" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10490,10 +10512,10 @@
     </row>
     <row r="7" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="34" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10501,7 +10523,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10509,22 +10531,22 @@
         <v>86</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="36" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="37" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10544,17 +10566,17 @@
     </row>
     <row r="17" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="38" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="39" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C19" s="40" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11564,26 +11586,26 @@
     <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="37" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="33" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="37" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="41" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Atualizado o excel de relatório de acessibilidade
</commit_message>
<xml_diff>
--- a/documento_projeto/Pixels - Relatório de Acessibilidade.xlsx
+++ b/documento_projeto/Pixels - Relatório de Acessibilidade.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Fatec\pixels\documento_projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50419C1A-7D31-4688-8B4A-19A8C451A53A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7671CD0B-1C54-4245-BF9C-1D7CC0B67FEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8730" yWindow="1575" windowWidth="17730" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Relatório" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="172">
   <si>
     <t>ID</t>
   </si>
@@ -707,7 +707,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -738,9 +738,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -806,9 +803,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -858,6 +852,23 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1244,10 +1255,10 @@
   <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1514,28 +1525,28 @@
       <c r="E6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="52" t="s">
+      <c r="F6" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="52" t="s">
+      <c r="G6" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="54" t="s">
+      <c r="H6" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="53" t="s">
+      <c r="I6" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="52" t="s">
+      <c r="J6" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="52" t="s">
+      <c r="K6" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="55">
+      <c r="L6" s="53">
         <v>44126</v>
       </c>
-      <c r="M6" s="52" t="s">
+      <c r="M6" s="50" t="s">
         <v>35</v>
       </c>
       <c r="N6" s="2" t="s">
@@ -1547,7 +1558,7 @@
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>47</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -1568,7 +1579,7 @@
       <c r="H7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="13" t="s">
         <v>50</v>
       </c>
       <c r="J7" s="2" t="s">
@@ -1604,7 +1615,7 @@
       <c r="E8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="14" t="s">
         <v>51</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -1685,7 +1696,7 @@
       <c r="B10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="54" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -1862,7 +1873,7 @@
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>47</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -2015,10 +2026,10 @@
       <c r="G17" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="H17" s="12" t="s">
+      <c r="H17" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="I17" s="12" t="s">
+      <c r="I17" s="11" t="s">
         <v>31</v>
       </c>
       <c r="J17" s="10" t="s">
@@ -2027,7 +2038,7 @@
       <c r="K17" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="L17" s="16"/>
+      <c r="L17" s="15"/>
       <c r="M17" s="10" t="s">
         <v>73</v>
       </c>
@@ -2056,10 +2067,10 @@
       <c r="G18" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="H18" s="12" t="s">
+      <c r="H18" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="I18" s="12" t="s">
+      <c r="I18" s="11" t="s">
         <v>31</v>
       </c>
       <c r="J18" s="10" t="s">
@@ -2068,11 +2079,11 @@
       <c r="K18" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="L18" s="16"/>
+      <c r="L18" s="15"/>
       <c r="M18" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="N18" s="17"/>
+      <c r="N18" s="16"/>
       <c r="O18" s="5"/>
     </row>
     <row r="19" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2124,7 +2135,7 @@
       <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="12" t="s">
         <v>47</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -2214,7 +2225,7 @@
       <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="12" t="s">
         <v>47</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -2232,10 +2243,10 @@
       <c r="G22" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="H22" s="12" t="s">
+      <c r="H22" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="I22" s="12" t="s">
+      <c r="I22" s="11" t="s">
         <v>82</v>
       </c>
       <c r="J22" s="10" t="s">
@@ -2244,7 +2255,7 @@
       <c r="K22" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="L22" s="16"/>
+      <c r="L22" s="15"/>
       <c r="M22" s="10" t="s">
         <v>35</v>
       </c>
@@ -2255,7 +2266,7 @@
       <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="12" t="s">
         <v>47</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -2330,7 +2341,7 @@
       <c r="K24" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="L24" s="18"/>
+      <c r="L24" s="17"/>
       <c r="M24" s="2" t="s">
         <v>63</v>
       </c>
@@ -2343,28 +2354,28 @@
       <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="18" t="s">
         <v>15</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="E25" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="F25" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="G25" s="22" t="s">
+      <c r="G25" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="H25" s="23" t="s">
+      <c r="H25" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="I25" s="23" t="s">
+      <c r="I25" s="22" t="s">
         <v>22</v>
       </c>
       <c r="J25" s="2" t="s">
@@ -2373,55 +2384,55 @@
       <c r="K25" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="L25" s="24"/>
-      <c r="M25" s="22" t="s">
+      <c r="L25" s="23"/>
+      <c r="M25" s="21" t="s">
         <v>25</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="O25" s="22"/>
+      <c r="O25" s="21"/>
     </row>
     <row r="26" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="24" t="s">
         <v>47</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="26" t="s">
+      <c r="D26" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="E26" s="27" t="s">
+      <c r="E26" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="F26" s="28" t="s">
+      <c r="F26" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="G26" s="28" t="s">
+      <c r="G26" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H26" s="29" t="s">
+      <c r="H26" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="I26" s="29" t="s">
+      <c r="I26" s="28" t="s">
         <v>91</v>
       </c>
       <c r="J26" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K26" s="28" t="s">
+      <c r="K26" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="L26" s="30"/>
-      <c r="M26" s="28" t="s">
+      <c r="L26" s="29"/>
+      <c r="M26" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="N26" s="28"/>
-      <c r="O26" s="31" t="s">
+      <c r="N26" s="27"/>
+      <c r="O26" s="30" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2429,46 +2440,46 @@
       <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="31" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="E27" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="F27" s="22" t="s">
+      <c r="F27" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="G27" s="22" t="s">
+      <c r="G27" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="H27" s="23" t="s">
+      <c r="H27" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="I27" s="23" t="s">
+      <c r="I27" s="22" t="s">
         <v>31</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K27" s="22" t="s">
+      <c r="K27" s="21" t="s">
         <v>92</v>
       </c>
       <c r="L27" s="9">
         <v>44126</v>
       </c>
-      <c r="M27" s="22" t="s">
+      <c r="M27" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="N27" s="22" t="s">
+      <c r="N27" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="O27" s="31" t="s">
+      <c r="O27" s="30" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2476,46 +2487,46 @@
       <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="31" t="s">
         <v>26</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E28" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="F28" s="22" t="s">
+      <c r="F28" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="G28" s="22" t="s">
+      <c r="G28" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="H28" s="23" t="s">
+      <c r="H28" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="I28" s="23" t="s">
+      <c r="I28" s="22" t="s">
         <v>31</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K28" s="22" t="s">
+      <c r="K28" s="21" t="s">
         <v>92</v>
       </c>
       <c r="L28" s="9">
         <v>44126</v>
       </c>
-      <c r="M28" s="22" t="s">
+      <c r="M28" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="N28" s="22" t="s">
+      <c r="N28" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="O28" s="31" t="s">
+      <c r="O28" s="30" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2523,46 +2534,46 @@
       <c r="A29" s="2">
         <v>28</v>
       </c>
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="31" t="s">
         <v>26</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="E29" s="21" t="s">
+      <c r="E29" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="F29" s="22" t="s">
+      <c r="F29" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="G29" s="22" t="s">
+      <c r="G29" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="H29" s="23" t="s">
+      <c r="H29" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="I29" s="23" t="s">
+      <c r="I29" s="22" t="s">
         <v>31</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K29" s="22" t="s">
+      <c r="K29" s="21" t="s">
         <v>92</v>
       </c>
       <c r="L29" s="9">
         <v>44126</v>
       </c>
-      <c r="M29" s="22" t="s">
+      <c r="M29" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="N29" s="22" t="s">
+      <c r="N29" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="O29" s="31" t="s">
+      <c r="O29" s="30" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2570,42 +2581,42 @@
       <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="B30" s="32" t="s">
+      <c r="B30" s="31" t="s">
         <v>26</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D30" s="26" t="s">
+      <c r="D30" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="E30" s="27" t="s">
+      <c r="E30" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="F30" s="28" t="s">
+      <c r="F30" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="G30" s="28" t="s">
+      <c r="G30" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="H30" s="29" t="s">
+      <c r="H30" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="I30" s="29" t="s">
+      <c r="I30" s="28" t="s">
         <v>31</v>
       </c>
       <c r="J30" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K30" s="28" t="s">
+      <c r="K30" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="L30" s="33"/>
-      <c r="M30" s="28" t="s">
+      <c r="L30" s="32"/>
+      <c r="M30" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="N30" s="28"/>
-      <c r="O30" s="31" t="s">
+      <c r="N30" s="27"/>
+      <c r="O30" s="30" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2613,124 +2624,124 @@
       <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="B31" s="32" t="s">
+      <c r="B31" s="31" t="s">
         <v>26</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D31" s="26" t="s">
+      <c r="D31" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="E31" s="27" t="s">
+      <c r="E31" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="F31" s="28" t="s">
+      <c r="F31" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="G31" s="28" t="s">
+      <c r="G31" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="H31" s="29" t="s">
+      <c r="H31" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="I31" s="29" t="s">
+      <c r="I31" s="28" t="s">
         <v>82</v>
       </c>
       <c r="J31" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K31" s="28" t="s">
+      <c r="K31" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="L31" s="34"/>
-      <c r="M31" s="28" t="s">
+      <c r="L31" s="33"/>
+      <c r="M31" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="N31" s="28"/>
-      <c r="O31" s="35"/>
+      <c r="N31" s="27"/>
+      <c r="O31" s="34"/>
     </row>
     <row r="32" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="31" t="s">
         <v>26</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D32" s="26" t="s">
+      <c r="D32" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="E32" s="27" t="s">
+      <c r="E32" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="F32" s="28" t="s">
+      <c r="F32" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="G32" s="28" t="s">
+      <c r="G32" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="H32" s="36" t="s">
+      <c r="H32" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="I32" s="29" t="s">
+      <c r="I32" s="28" t="s">
         <v>82</v>
       </c>
       <c r="J32" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K32" s="28" t="s">
+      <c r="K32" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="L32" s="37"/>
-      <c r="M32" s="28" t="s">
+      <c r="L32" s="36"/>
+      <c r="M32" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N32" s="28"/>
-      <c r="O32" s="35"/>
+      <c r="N32" s="27"/>
+      <c r="O32" s="34"/>
     </row>
     <row r="33" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="31" t="s">
         <v>26</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D33" s="26" t="s">
+      <c r="D33" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="E33" s="27" t="s">
+      <c r="E33" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="F33" s="28" t="s">
+      <c r="F33" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="G33" s="28" t="s">
+      <c r="G33" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="H33" s="36" t="s">
+      <c r="H33" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="I33" s="29" t="s">
+      <c r="I33" s="28" t="s">
         <v>82</v>
       </c>
       <c r="J33" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K33" s="28" t="s">
+      <c r="K33" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="L33" s="37"/>
-      <c r="M33" s="28" t="s">
+      <c r="L33" s="36"/>
+      <c r="M33" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N33" s="28"/>
-      <c r="O33" s="35"/>
+      <c r="N33" s="27"/>
+      <c r="O33" s="34"/>
     </row>
     <row r="34" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
@@ -2742,35 +2753,35 @@
       <c r="C34" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="52" t="s">
+      <c r="D34" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="E34" s="52" t="s">
+      <c r="E34" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="F34" s="52" t="s">
+      <c r="F34" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="G34" s="52" t="s">
+      <c r="G34" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="H34" s="53" t="s">
+      <c r="H34" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="I34" s="53" t="s">
+      <c r="I34" s="51" t="s">
         <v>109</v>
       </c>
-      <c r="J34" s="52" t="s">
+      <c r="J34" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="K34" s="52" t="s">
+      <c r="K34" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="L34" s="52"/>
-      <c r="M34" s="52" t="s">
+      <c r="L34" s="50"/>
+      <c r="M34" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="N34" s="52" t="s">
+      <c r="N34" s="50" t="s">
         <v>25</v>
       </c>
       <c r="O34" s="5"/>
@@ -2779,42 +2790,42 @@
       <c r="A35" s="2">
         <v>34</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D35" s="26" t="s">
+      <c r="C35" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="E35" s="27" t="s">
+      <c r="E35" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="F35" s="28" t="s">
+      <c r="F35" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="G35" s="28" t="s">
+      <c r="G35" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H35" s="29" t="s">
+      <c r="H35" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="I35" s="29" t="s">
+      <c r="I35" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="J35" s="10" t="s">
+      <c r="J35" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="K35" s="10" t="s">
+      <c r="K35" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="L35" s="34"/>
-      <c r="M35" s="28" t="s">
+      <c r="L35" s="59"/>
+      <c r="M35" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="N35" s="10"/>
-      <c r="O35" s="22"/>
+      <c r="N35" s="50"/>
+      <c r="O35" s="21"/>
     </row>
     <row r="36" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
@@ -2823,38 +2834,38 @@
       <c r="B36" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D36" s="10" t="s">
+      <c r="C36" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="F36" s="10" t="s">
+      <c r="F36" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="G36" s="10" t="s">
+      <c r="G36" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="H36" s="12" t="s">
+      <c r="H36" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="I36" s="12" t="s">
+      <c r="I36" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="J36" s="10" t="s">
+      <c r="J36" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="K36" s="10" t="s">
+      <c r="K36" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="L36" s="38"/>
-      <c r="M36" s="10" t="s">
+      <c r="L36" s="60"/>
+      <c r="M36" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="N36" s="10"/>
+      <c r="N36" s="50"/>
       <c r="O36" s="2"/>
     </row>
     <row r="37" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2879,17 +2890,17 @@
       <c r="G37" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H37" s="12" t="s">
+      <c r="H37" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="I37" s="12" t="s">
+      <c r="I37" s="11" t="s">
         <v>118</v>
       </c>
       <c r="J37" s="10" t="s">
         <v>92</v>
       </c>
       <c r="K37" s="10"/>
-      <c r="L37" s="16"/>
+      <c r="L37" s="15"/>
       <c r="M37" s="10"/>
       <c r="N37" s="10"/>
       <c r="O37" s="5"/>
@@ -2898,7 +2909,7 @@
       <c r="A38" s="2">
         <v>37</v>
       </c>
-      <c r="B38" s="32" t="s">
+      <c r="B38" s="31" t="s">
         <v>26</v>
       </c>
       <c r="C38" s="4" t="s">
@@ -2916,17 +2927,17 @@
       <c r="G38" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="H38" s="12" t="s">
+      <c r="H38" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="I38" s="12" t="s">
+      <c r="I38" s="11" t="s">
         <v>122</v>
       </c>
       <c r="J38" s="10" t="s">
         <v>92</v>
       </c>
       <c r="K38" s="10"/>
-      <c r="L38" s="16"/>
+      <c r="L38" s="15"/>
       <c r="M38" s="10"/>
       <c r="N38" s="10"/>
       <c r="O38" s="5"/>
@@ -2935,7 +2946,7 @@
       <c r="A39" s="2">
         <v>38</v>
       </c>
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="31" t="s">
         <v>26</v>
       </c>
       <c r="C39" s="4" t="s">
@@ -2953,17 +2964,17 @@
       <c r="G39" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="H39" s="12" t="s">
+      <c r="H39" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="I39" s="12" t="s">
+      <c r="I39" s="11" t="s">
         <v>125</v>
       </c>
       <c r="J39" s="10" t="s">
         <v>92</v>
       </c>
       <c r="K39" s="10"/>
-      <c r="L39" s="16"/>
+      <c r="L39" s="15"/>
       <c r="M39" s="10"/>
       <c r="N39" s="10"/>
       <c r="O39" s="5"/>
@@ -2972,7 +2983,7 @@
       <c r="A40" s="2">
         <v>39</v>
       </c>
-      <c r="B40" s="32" t="s">
+      <c r="B40" s="31" t="s">
         <v>26</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -2990,17 +3001,17 @@
       <c r="G40" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="H40" s="12" t="s">
+      <c r="H40" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="I40" s="12" t="s">
+      <c r="I40" s="11" t="s">
         <v>128</v>
       </c>
       <c r="J40" s="10" t="s">
         <v>92</v>
       </c>
       <c r="K40" s="10"/>
-      <c r="L40" s="16"/>
+      <c r="L40" s="15"/>
       <c r="M40" s="10"/>
       <c r="N40" s="10"/>
       <c r="O40" s="5"/>
@@ -3009,7 +3020,7 @@
       <c r="A41" s="2">
         <v>40</v>
       </c>
-      <c r="B41" s="25" t="s">
+      <c r="B41" s="24" t="s">
         <v>47</v>
       </c>
       <c r="C41" s="4" t="s">
@@ -3027,15 +3038,15 @@
       <c r="G41" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="H41" s="12" t="s">
+      <c r="H41" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="I41" s="12"/>
+      <c r="I41" s="11"/>
       <c r="J41" s="10" t="s">
         <v>92</v>
       </c>
       <c r="K41" s="10"/>
-      <c r="L41" s="16"/>
+      <c r="L41" s="15"/>
       <c r="M41" s="10"/>
       <c r="N41" s="10"/>
       <c r="O41" s="5"/>
@@ -3044,7 +3055,7 @@
       <c r="A42" s="2">
         <v>41</v>
       </c>
-      <c r="B42" s="25" t="s">
+      <c r="B42" s="24" t="s">
         <v>47</v>
       </c>
       <c r="C42" s="4" t="s">
@@ -3062,17 +3073,17 @@
       <c r="G42" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="H42" s="12" t="s">
+      <c r="H42" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="I42" s="12" t="s">
+      <c r="I42" s="11" t="s">
         <v>135</v>
       </c>
       <c r="J42" s="10" t="s">
         <v>92</v>
       </c>
       <c r="K42" s="10"/>
-      <c r="L42" s="16"/>
+      <c r="L42" s="15"/>
       <c r="M42" s="10"/>
       <c r="N42" s="10"/>
       <c r="O42" s="5"/>
@@ -3099,17 +3110,17 @@
       <c r="G43" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="H43" s="12" t="s">
+      <c r="H43" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="I43" s="12" t="s">
+      <c r="I43" s="11" t="s">
         <v>139</v>
       </c>
       <c r="J43" s="10" t="s">
         <v>92</v>
       </c>
       <c r="K43" s="10"/>
-      <c r="L43" s="16"/>
+      <c r="L43" s="15"/>
       <c r="M43" s="10"/>
       <c r="N43" s="10"/>
       <c r="O43" s="5"/>
@@ -3118,7 +3129,7 @@
       <c r="A44" s="2">
         <v>43</v>
       </c>
-      <c r="B44" s="32" t="s">
+      <c r="B44" s="31" t="s">
         <v>26</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -3136,17 +3147,17 @@
       <c r="G44" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="H44" s="12" t="s">
+      <c r="H44" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="I44" s="12" t="s">
+      <c r="I44" s="11" t="s">
         <v>143</v>
       </c>
       <c r="J44" s="10" t="s">
         <v>92</v>
       </c>
       <c r="K44" s="10"/>
-      <c r="L44" s="16"/>
+      <c r="L44" s="15"/>
       <c r="M44" s="10"/>
       <c r="N44" s="10"/>
       <c r="O44" s="5"/>
@@ -3155,16 +3166,16 @@
       <c r="A45" s="2">
         <v>44</v>
       </c>
-      <c r="B45" s="25" t="s">
+      <c r="B45" s="24" t="s">
         <v>47</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D45" s="26" t="s">
+      <c r="D45" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="E45" s="27" t="s">
+      <c r="E45" s="26" t="s">
         <v>84</v>
       </c>
       <c r="F45" s="10" t="s">
@@ -3173,37 +3184,37 @@
       <c r="G45" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H45" s="12" t="s">
+      <c r="H45" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="I45" s="12" t="s">
+      <c r="I45" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="J45" s="39">
+      <c r="J45" s="37">
         <v>43840</v>
       </c>
       <c r="K45" s="10"/>
-      <c r="L45" s="16"/>
+      <c r="L45" s="15"/>
       <c r="M45" s="10" t="s">
         <v>63</v>
       </c>
       <c r="N45" s="10"/>
-      <c r="O45" s="5"/>
+      <c r="O45" s="61"/>
     </row>
     <row r="46" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
-      <c r="B46" s="25" t="s">
+      <c r="B46" s="24" t="s">
         <v>47</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D46" s="26" t="s">
+      <c r="D46" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="E46" s="27" t="s">
+      <c r="E46" s="26" t="s">
         <v>84</v>
       </c>
       <c r="F46" s="10" t="s">
@@ -3212,17 +3223,17 @@
       <c r="G46" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H46" s="12" t="s">
+      <c r="H46" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="I46" s="12" t="s">
+      <c r="I46" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="J46" s="39">
+      <c r="J46" s="37">
         <v>43840</v>
       </c>
       <c r="K46" s="10"/>
-      <c r="L46" s="16"/>
+      <c r="L46" s="15"/>
       <c r="M46" s="10" t="s">
         <v>63</v>
       </c>
@@ -3233,16 +3244,16 @@
       <c r="A47" s="2">
         <v>46</v>
       </c>
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="24" t="s">
         <v>47</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D47" s="26" t="s">
+      <c r="D47" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="E47" s="27" t="s">
+      <c r="E47" s="26" t="s">
         <v>84</v>
       </c>
       <c r="F47" s="10" t="s">
@@ -3251,17 +3262,17 @@
       <c r="G47" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H47" s="12" t="s">
+      <c r="H47" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="I47" s="12" t="s">
+      <c r="I47" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="J47" s="39">
+      <c r="J47" s="37">
         <v>43840</v>
       </c>
       <c r="K47" s="10"/>
-      <c r="L47" s="16"/>
+      <c r="L47" s="15"/>
       <c r="M47" s="10" t="s">
         <v>63</v>
       </c>
@@ -3272,16 +3283,16 @@
       <c r="A48" s="2">
         <v>47</v>
       </c>
-      <c r="B48" s="25" t="s">
+      <c r="B48" s="24" t="s">
         <v>47</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D48" s="26" t="s">
+      <c r="D48" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="E48" s="27" t="s">
+      <c r="E48" s="26" t="s">
         <v>84</v>
       </c>
       <c r="F48" s="10" t="s">
@@ -3290,17 +3301,17 @@
       <c r="G48" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H48" s="12" t="s">
+      <c r="H48" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="I48" s="12" t="s">
+      <c r="I48" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="J48" s="39">
+      <c r="J48" s="37">
         <v>43840</v>
       </c>
       <c r="K48" s="10"/>
-      <c r="L48" s="16"/>
+      <c r="L48" s="15"/>
       <c r="M48" s="10" t="s">
         <v>63</v>
       </c>
@@ -3314,38 +3325,42 @@
       <c r="B49" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D49" s="10" t="s">
+      <c r="C49" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D49" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="E49" s="10" t="s">
+      <c r="E49" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="F49" s="10" t="s">
+      <c r="F49" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="G49" s="10" t="s">
+      <c r="G49" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="H49" s="12" t="s">
+      <c r="H49" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="I49" s="12" t="s">
+      <c r="I49" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="J49" s="10" t="s">
+      <c r="J49" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="K49" s="10" t="s">
+      <c r="K49" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="L49" s="10"/>
-      <c r="M49" s="10" t="s">
+      <c r="L49" s="53">
+        <v>44126</v>
+      </c>
+      <c r="M49" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="N49" s="10"/>
+      <c r="N49" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="O49" s="5"/>
     </row>
     <row r="50" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3355,38 +3370,42 @@
       <c r="B50" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C50" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D50" s="10" t="s">
+      <c r="C50" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D50" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="E50" s="10" t="s">
+      <c r="E50" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="F50" s="10" t="s">
+      <c r="F50" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="G50" s="10" t="s">
+      <c r="G50" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="H50" s="12" t="s">
+      <c r="H50" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="I50" s="12" t="s">
+      <c r="I50" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="J50" s="10" t="s">
+      <c r="J50" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="K50" s="10" t="s">
+      <c r="K50" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="L50" s="10"/>
-      <c r="M50" s="10" t="s">
+      <c r="L50" s="53">
+        <v>44126</v>
+      </c>
+      <c r="M50" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="N50" s="10"/>
+      <c r="N50" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="O50" s="5"/>
     </row>
     <row r="51" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3441,79 +3460,87 @@
       <c r="B52" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D52" s="10" t="s">
+      <c r="C52" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D52" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="E52" s="10" t="s">
+      <c r="E52" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="F52" s="10" t="s">
+      <c r="F52" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="G52" s="10" t="s">
+      <c r="G52" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="H52" s="11" t="s">
+      <c r="H52" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="I52" s="12" t="s">
+      <c r="I52" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="J52" s="10" t="s">
+      <c r="J52" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="K52" s="10" t="s">
+      <c r="K52" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="L52" s="10"/>
-      <c r="M52" s="10" t="s">
+      <c r="L52" s="53">
+        <v>44126</v>
+      </c>
+      <c r="M52" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="N52" s="10"/>
+      <c r="N52" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="O52" s="5"/>
     </row>
     <row r="53" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>52</v>
       </c>
-      <c r="B53" s="13" t="s">
+      <c r="B53" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D53" s="10" t="s">
+      <c r="C53" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D53" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="E53" s="10" t="s">
+      <c r="E53" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="F53" s="10" t="s">
+      <c r="F53" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="G53" s="10" t="s">
+      <c r="G53" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="H53" s="12" t="s">
+      <c r="H53" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="I53" s="11" t="s">
+      <c r="I53" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="J53" s="10" t="s">
+      <c r="J53" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="K53" s="10" t="s">
+      <c r="K53" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="L53" s="10"/>
-      <c r="M53" s="10" t="s">
+      <c r="L53" s="53">
+        <v>44126</v>
+      </c>
+      <c r="M53" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N53" s="10"/>
+      <c r="N53" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="O53" s="5"/>
     </row>
     <row r="54" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3532,16 +3559,16 @@
       <c r="E54" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="F54" s="40" t="s">
+      <c r="F54" s="38" t="s">
         <v>51</v>
       </c>
       <c r="G54" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H54" s="12" t="s">
+      <c r="H54" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="I54" s="12" t="s">
+      <c r="I54" s="11" t="s">
         <v>31</v>
       </c>
       <c r="J54" s="10" t="s">
@@ -3550,7 +3577,7 @@
       <c r="K54" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="L54" s="16"/>
+      <c r="L54" s="15"/>
       <c r="M54" s="10" t="s">
         <v>25</v>
       </c>
@@ -3579,10 +3606,10 @@
       <c r="G55" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H55" s="12" t="s">
+      <c r="H55" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="I55" s="12" t="s">
+      <c r="I55" s="11" t="s">
         <v>31</v>
       </c>
       <c r="J55" s="10" t="s">
@@ -3591,7 +3618,7 @@
       <c r="K55" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="L55" s="16"/>
+      <c r="L55" s="15"/>
       <c r="M55" s="10" t="s">
         <v>25</v>
       </c>
@@ -3620,10 +3647,10 @@
       <c r="G56" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="H56" s="12" t="s">
+      <c r="H56" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="I56" s="12" t="s">
+      <c r="I56" s="11" t="s">
         <v>46</v>
       </c>
       <c r="J56" s="10" t="s">
@@ -3632,7 +3659,7 @@
       <c r="K56" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="L56" s="16"/>
+      <c r="L56" s="15"/>
       <c r="M56" s="10" t="s">
         <v>25</v>
       </c>
@@ -3661,10 +3688,10 @@
       <c r="G57" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="H57" s="12" t="s">
+      <c r="H57" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="I57" s="12" t="s">
+      <c r="I57" s="11" t="s">
         <v>57</v>
       </c>
       <c r="J57" s="10" t="s">
@@ -3673,7 +3700,7 @@
       <c r="K57" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="L57" s="16"/>
+      <c r="L57" s="15"/>
       <c r="M57" s="10" t="s">
         <v>25</v>
       </c>
@@ -3702,10 +3729,10 @@
       <c r="G58" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="H58" s="12" t="s">
+      <c r="H58" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="I58" s="12" t="s">
+      <c r="I58" s="11" t="s">
         <v>57</v>
       </c>
       <c r="J58" s="10" t="s">
@@ -3714,7 +3741,7 @@
       <c r="K58" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="L58" s="16"/>
+      <c r="L58" s="15"/>
       <c r="M58" s="10" t="s">
         <v>25</v>
       </c>
@@ -3743,10 +3770,10 @@
       <c r="G59" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="H59" s="12" t="s">
+      <c r="H59" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="I59" s="12" t="s">
+      <c r="I59" s="11" t="s">
         <v>62</v>
       </c>
       <c r="J59" s="10" t="s">
@@ -3755,7 +3782,7 @@
       <c r="K59" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="L59" s="16"/>
+      <c r="L59" s="15"/>
       <c r="M59" s="10" t="s">
         <v>63</v>
       </c>
@@ -3766,7 +3793,7 @@
       <c r="A60" s="2">
         <v>59</v>
       </c>
-      <c r="B60" s="13" t="s">
+      <c r="B60" s="12" t="s">
         <v>47</v>
       </c>
       <c r="C60" s="4" t="s">
@@ -3784,10 +3811,10 @@
       <c r="G60" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="H60" s="12" t="s">
+      <c r="H60" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="I60" s="12" t="s">
+      <c r="I60" s="11" t="s">
         <v>62</v>
       </c>
       <c r="J60" s="10" t="s">
@@ -3796,7 +3823,7 @@
       <c r="K60" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="L60" s="16"/>
+      <c r="L60" s="15"/>
       <c r="M60" s="10" t="s">
         <v>63</v>
       </c>
@@ -3825,10 +3852,10 @@
       <c r="G61" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="H61" s="12" t="s">
+      <c r="H61" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="I61" s="12" t="s">
+      <c r="I61" s="11" t="s">
         <v>57</v>
       </c>
       <c r="J61" s="10" t="s">
@@ -3837,7 +3864,7 @@
       <c r="K61" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="L61" s="16"/>
+      <c r="L61" s="15"/>
       <c r="M61" s="10" t="s">
         <v>63</v>
       </c>
@@ -3866,10 +3893,10 @@
       <c r="G62" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="H62" s="12" t="s">
+      <c r="H62" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="I62" s="12" t="s">
+      <c r="I62" s="11" t="s">
         <v>62</v>
       </c>
       <c r="J62" s="10" t="s">
@@ -3878,7 +3905,7 @@
       <c r="K62" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="L62" s="16"/>
+      <c r="L62" s="15"/>
       <c r="M62" s="10" t="s">
         <v>63</v>
       </c>
@@ -3907,10 +3934,10 @@
       <c r="G63" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="H63" s="12" t="s">
+      <c r="H63" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="I63" s="12" t="s">
+      <c r="I63" s="11" t="s">
         <v>31</v>
       </c>
       <c r="J63" s="10" t="s">
@@ -3919,7 +3946,7 @@
       <c r="K63" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="L63" s="16"/>
+      <c r="L63" s="15"/>
       <c r="M63" s="10" t="s">
         <v>73</v>
       </c>
@@ -3948,10 +3975,10 @@
       <c r="G64" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="H64" s="12" t="s">
+      <c r="H64" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="I64" s="12" t="s">
+      <c r="I64" s="11" t="s">
         <v>31</v>
       </c>
       <c r="J64" s="10" t="s">
@@ -3960,7 +3987,7 @@
       <c r="K64" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="L64" s="16"/>
+      <c r="L64" s="15"/>
       <c r="M64" s="10" t="s">
         <v>73</v>
       </c>
@@ -3974,45 +4001,49 @@
       <c r="B65" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C65" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D65" s="10" t="s">
+      <c r="C65" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D65" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="10" t="s">
+      <c r="E65" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="F65" s="10" t="s">
+      <c r="F65" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G65" s="10" t="s">
+      <c r="G65" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H65" s="12" t="s">
+      <c r="H65" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="I65" s="12" t="s">
+      <c r="I65" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J65" s="10" t="s">
+      <c r="J65" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K65" s="10" t="s">
+      <c r="K65" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="L65" s="16"/>
-      <c r="M65" s="10" t="s">
+      <c r="L65" s="9">
+        <v>44118</v>
+      </c>
+      <c r="M65" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N65" s="10"/>
+      <c r="N65" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="O65" s="5"/>
     </row>
     <row r="66" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>65</v>
       </c>
-      <c r="B66" s="13" t="s">
+      <c r="B66" s="12" t="s">
         <v>47</v>
       </c>
       <c r="C66" s="8" t="s">
@@ -4102,7 +4133,7 @@
       <c r="A68" s="2">
         <v>67</v>
       </c>
-      <c r="B68" s="13" t="s">
+      <c r="B68" s="12" t="s">
         <v>47</v>
       </c>
       <c r="C68" s="4" t="s">
@@ -4120,10 +4151,10 @@
       <c r="G68" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="H68" s="12" t="s">
+      <c r="H68" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="I68" s="12" t="s">
+      <c r="I68" s="11" t="s">
         <v>82</v>
       </c>
       <c r="J68" s="10" t="s">
@@ -4132,7 +4163,7 @@
       <c r="K68" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="L68" s="16"/>
+      <c r="L68" s="15"/>
       <c r="M68" s="10" t="s">
         <v>35</v>
       </c>
@@ -4143,7 +4174,7 @@
       <c r="A69" s="2">
         <v>68</v>
       </c>
-      <c r="B69" s="13" t="s">
+      <c r="B69" s="12" t="s">
         <v>47</v>
       </c>
       <c r="C69" s="8" t="s">
@@ -5140,26 +5171,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="42"/>
+      <c r="C1" s="40"/>
     </row>
     <row r="2" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44" t="s">
+      <c r="C2" s="41"/>
+      <c r="D2" s="42" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="44" t="s">
+      <c r="C3" s="41"/>
+      <c r="D3" s="42" t="s">
         <v>155</v>
       </c>
     </row>
@@ -5167,13 +5198,13 @@
       <c r="B4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="44" t="s">
+      <c r="C4" s="41"/>
+      <c r="D4" s="42" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="39" t="s">
         <v>2</v>
       </c>
     </row>
@@ -5181,66 +5212,66 @@
       <c r="B7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="42" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="43" t="s">
         <v>158</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="42" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="42" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="D10" s="42" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="46" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="47" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="47" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="47" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="17" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C17" s="49" t="s">
+      <c r="C17" s="47" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="18" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="47" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="19" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C19" s="50" t="s">
+      <c r="C19" s="48" t="s">
         <v>166</v>
       </c>
     </row>
@@ -6251,25 +6282,25 @@
     <row r="1" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="46" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="42" t="s">
         <v>168</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="49" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="46" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="49" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>

<commit_message>
atualização de planilhas e doc word
</commit_message>
<xml_diff>
--- a/documento_projeto/Pixels - Relatório de Acessibilidade.xlsx
+++ b/documento_projeto/Pixels - Relatório de Acessibilidade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp1\htdocs\pixels\documento_projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCA9F3F-8AF5-476C-8CF9-D4B051139BFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE67A27-D1E7-4B68-ACDC-19D2383AF568}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="193">
   <si>
     <t>ID</t>
   </si>
@@ -636,7 +636,7 @@
     <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="166" formatCode="d/m/yyyy\ h:mm:ss"/>
     <numFmt numFmtId="167" formatCode="&quot;R$ &quot;#,##0.00"/>
-    <numFmt numFmtId="171" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="168" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -1082,7 +1082,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1101,7 +1101,7 @@
     <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1110,10 +1110,10 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1156,13 +1156,13 @@
     <xf numFmtId="2" fontId="3" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="2" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1566,10 +1566,10 @@
   <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="G56" sqref="G55:G56"/>
+      <selection pane="bottomRight" activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2750,7 +2750,9 @@
       <c r="M26" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="N26" s="25"/>
+      <c r="N26" s="25" t="s">
+        <v>25</v>
+      </c>
       <c r="O26" s="28" t="s">
         <v>93</v>
       </c>
@@ -5516,7 +5518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CFCABBE-0E49-485E-803F-BC21345278E9}">
   <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
@@ -5596,7 +5598,7 @@
         <v>400</v>
       </c>
       <c r="J2" s="80">
-        <f>(I2/60)*G2</f>
+        <f t="shared" ref="J2:J33" si="0">(I2/60)*G2</f>
         <v>500</v>
       </c>
     </row>
@@ -5623,14 +5625,14 @@
         <v>52.5</v>
       </c>
       <c r="H3" s="87">
-        <f t="shared" ref="H3:H66" si="0">(E3/60)*G3</f>
+        <f t="shared" ref="H3:H66" si="1">(E3/60)*G3</f>
         <v>52.5</v>
       </c>
       <c r="I3" s="2">
         <v>50</v>
       </c>
       <c r="J3" s="80">
-        <f>(I3/60)*G3</f>
+        <f t="shared" si="0"/>
         <v>43.75</v>
       </c>
     </row>
@@ -5657,14 +5659,14 @@
         <v>52.5</v>
       </c>
       <c r="H4" s="87">
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="I4" s="2">
+        <v>10</v>
+      </c>
+      <c r="J4" s="80">
         <f t="shared" si="0"/>
-        <v>8.75</v>
-      </c>
-      <c r="I4" s="2">
-        <v>10</v>
-      </c>
-      <c r="J4" s="80">
-        <f>(I4/60)*G4</f>
         <v>8.75</v>
       </c>
     </row>
@@ -5691,14 +5693,14 @@
         <v>52.5</v>
       </c>
       <c r="H5" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
       <c r="I5" s="2">
         <v>18</v>
       </c>
       <c r="J5" s="80">
-        <f>(I5/60)*G5</f>
+        <f t="shared" si="0"/>
         <v>15.75</v>
       </c>
     </row>
@@ -5725,14 +5727,14 @@
         <v>52.5</v>
       </c>
       <c r="H6" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.5</v>
       </c>
       <c r="I6" s="2">
         <v>2</v>
       </c>
       <c r="J6" s="80">
-        <f>(I6/60)*G6</f>
+        <f t="shared" si="0"/>
         <v>1.75</v>
       </c>
     </row>
@@ -5759,14 +5761,14 @@
         <v>75</v>
       </c>
       <c r="H7" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.5</v>
       </c>
       <c r="I7" s="2">
         <v>20</v>
       </c>
       <c r="J7" s="80">
-        <f>(I7/60)*G7</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
@@ -5793,14 +5795,14 @@
         <v>52.5</v>
       </c>
       <c r="H8" s="87">
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="I8" s="2">
+        <v>10</v>
+      </c>
+      <c r="J8" s="80">
         <f t="shared" si="0"/>
-        <v>8.75</v>
-      </c>
-      <c r="I8" s="2">
-        <v>10</v>
-      </c>
-      <c r="J8" s="80">
-        <f>(I8/60)*G8</f>
         <v>8.75</v>
       </c>
     </row>
@@ -5827,14 +5829,14 @@
         <v>52.5</v>
       </c>
       <c r="H9" s="87">
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="I9" s="2">
+        <v>10</v>
+      </c>
+      <c r="J9" s="80">
         <f t="shared" si="0"/>
-        <v>8.75</v>
-      </c>
-      <c r="I9" s="2">
-        <v>10</v>
-      </c>
-      <c r="J9" s="80">
-        <f>(I9/60)*G9</f>
         <v>8.75</v>
       </c>
     </row>
@@ -5861,14 +5863,14 @@
         <v>52.5</v>
       </c>
       <c r="H10" s="87">
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="I10" s="2">
+        <v>10</v>
+      </c>
+      <c r="J10" s="80">
         <f t="shared" si="0"/>
-        <v>8.75</v>
-      </c>
-      <c r="I10" s="2">
-        <v>10</v>
-      </c>
-      <c r="J10" s="80">
-        <f>(I10/60)*G10</f>
         <v>8.75</v>
       </c>
     </row>
@@ -5895,14 +5897,14 @@
         <v>52.5</v>
       </c>
       <c r="H11" s="87">
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="I11" s="2">
+        <v>10</v>
+      </c>
+      <c r="J11" s="80">
         <f t="shared" si="0"/>
-        <v>8.75</v>
-      </c>
-      <c r="I11" s="2">
-        <v>10</v>
-      </c>
-      <c r="J11" s="80">
-        <f>(I11/60)*G11</f>
         <v>8.75</v>
       </c>
     </row>
@@ -5929,14 +5931,14 @@
         <v>52.5</v>
       </c>
       <c r="H12" s="87">
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="I12" s="2">
+        <v>10</v>
+      </c>
+      <c r="J12" s="80">
         <f t="shared" si="0"/>
-        <v>8.75</v>
-      </c>
-      <c r="I12" s="2">
-        <v>10</v>
-      </c>
-      <c r="J12" s="80">
-        <f>(I12/60)*G12</f>
         <v>8.75</v>
       </c>
     </row>
@@ -5963,14 +5965,14 @@
         <v>52.5</v>
       </c>
       <c r="H13" s="87">
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="I13" s="2">
+        <v>10</v>
+      </c>
+      <c r="J13" s="80">
         <f t="shared" si="0"/>
-        <v>8.75</v>
-      </c>
-      <c r="I13" s="2">
-        <v>10</v>
-      </c>
-      <c r="J13" s="80">
-        <f>(I13/60)*G13</f>
         <v>8.75</v>
       </c>
     </row>
@@ -5997,14 +5999,14 @@
         <v>52.5</v>
       </c>
       <c r="H14" s="87">
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="I14" s="2">
+        <v>10</v>
+      </c>
+      <c r="J14" s="80">
         <f t="shared" si="0"/>
-        <v>8.75</v>
-      </c>
-      <c r="I14" s="2">
-        <v>10</v>
-      </c>
-      <c r="J14" s="80">
-        <f>(I14/60)*G14</f>
         <v>8.75</v>
       </c>
     </row>
@@ -6031,14 +6033,14 @@
         <v>52.5</v>
       </c>
       <c r="H15" s="87">
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="I15" s="2">
+        <v>10</v>
+      </c>
+      <c r="J15" s="80">
         <f t="shared" si="0"/>
-        <v>8.75</v>
-      </c>
-      <c r="I15" s="2">
-        <v>10</v>
-      </c>
-      <c r="J15" s="80">
-        <f>(I15/60)*G15</f>
         <v>8.75</v>
       </c>
     </row>
@@ -6065,14 +6067,14 @@
         <v>52.5</v>
       </c>
       <c r="H16" s="87">
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="I16" s="2">
+        <v>10</v>
+      </c>
+      <c r="J16" s="80">
         <f t="shared" si="0"/>
-        <v>8.75</v>
-      </c>
-      <c r="I16" s="2">
-        <v>10</v>
-      </c>
-      <c r="J16" s="80">
-        <f>(I16/60)*G16</f>
         <v>8.75</v>
       </c>
     </row>
@@ -6099,14 +6101,14 @@
         <v>52.5</v>
       </c>
       <c r="H17" s="87">
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="I17" s="2">
+        <v>10</v>
+      </c>
+      <c r="J17" s="80">
         <f t="shared" si="0"/>
-        <v>8.75</v>
-      </c>
-      <c r="I17" s="2">
-        <v>10</v>
-      </c>
-      <c r="J17" s="80">
-        <f>(I17/60)*G17</f>
         <v>8.75</v>
       </c>
     </row>
@@ -6133,14 +6135,14 @@
         <v>52.5</v>
       </c>
       <c r="H18" s="87">
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="I18" s="2">
+        <v>10</v>
+      </c>
+      <c r="J18" s="80">
         <f t="shared" si="0"/>
-        <v>8.75</v>
-      </c>
-      <c r="I18" s="2">
-        <v>10</v>
-      </c>
-      <c r="J18" s="80">
-        <f>(I18/60)*G18</f>
         <v>8.75</v>
       </c>
     </row>
@@ -6167,14 +6169,14 @@
         <v>52.5</v>
       </c>
       <c r="H19" s="87">
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="I19" s="2">
+        <v>10</v>
+      </c>
+      <c r="J19" s="80">
         <f t="shared" si="0"/>
-        <v>8.75</v>
-      </c>
-      <c r="I19" s="2">
-        <v>10</v>
-      </c>
-      <c r="J19" s="80">
-        <f>(I19/60)*G19</f>
         <v>8.75</v>
       </c>
     </row>
@@ -6201,14 +6203,14 @@
         <v>52.5</v>
       </c>
       <c r="H20" s="87">
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="I20" s="2">
+        <v>10</v>
+      </c>
+      <c r="J20" s="80">
         <f t="shared" si="0"/>
-        <v>8.75</v>
-      </c>
-      <c r="I20" s="2">
-        <v>10</v>
-      </c>
-      <c r="J20" s="80">
-        <f>(I20/60)*G20</f>
         <v>8.75</v>
       </c>
     </row>
@@ -6235,14 +6237,14 @@
         <v>52.5</v>
       </c>
       <c r="H21" s="87">
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="I21" s="2">
+        <v>10</v>
+      </c>
+      <c r="J21" s="80">
         <f t="shared" si="0"/>
-        <v>8.75</v>
-      </c>
-      <c r="I21" s="2">
-        <v>10</v>
-      </c>
-      <c r="J21" s="80">
-        <f>(I21/60)*G21</f>
         <v>8.75</v>
       </c>
     </row>
@@ -6269,14 +6271,14 @@
         <v>75</v>
       </c>
       <c r="H22" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.75</v>
       </c>
       <c r="I22" s="2">
         <v>40</v>
       </c>
       <c r="J22" s="80">
-        <f>(I22/60)*G22</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
@@ -6303,14 +6305,14 @@
         <v>75</v>
       </c>
       <c r="H23" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.75</v>
       </c>
       <c r="I23" s="2">
         <v>30</v>
       </c>
       <c r="J23" s="80">
-        <f>(I23/60)*G23</f>
+        <f t="shared" si="0"/>
         <v>37.5</v>
       </c>
     </row>
@@ -6337,14 +6339,14 @@
         <v>75</v>
       </c>
       <c r="H24" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.75</v>
       </c>
       <c r="I24" s="2">
         <v>20</v>
       </c>
       <c r="J24" s="80">
-        <f>(I24/60)*G24</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
@@ -6371,14 +6373,14 @@
         <v>75</v>
       </c>
       <c r="H25" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.75</v>
       </c>
       <c r="I25" s="2">
         <v>20</v>
       </c>
       <c r="J25" s="80">
-        <f>(I25/60)*G25</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
@@ -6405,12 +6407,12 @@
         <v>52.5</v>
       </c>
       <c r="H26" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.5</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="80">
-        <f>(I26/60)*G26</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6437,14 +6439,14 @@
         <v>52.5</v>
       </c>
       <c r="H27" s="87">
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="I27" s="2">
+        <v>10</v>
+      </c>
+      <c r="J27" s="80">
         <f t="shared" si="0"/>
-        <v>8.75</v>
-      </c>
-      <c r="I27" s="2">
-        <v>10</v>
-      </c>
-      <c r="J27" s="80">
-        <f>(I27/60)*G27</f>
         <v>8.75</v>
       </c>
     </row>
@@ -6471,14 +6473,14 @@
         <v>52.5</v>
       </c>
       <c r="H28" s="87">
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="I28" s="2">
+        <v>10</v>
+      </c>
+      <c r="J28" s="80">
         <f t="shared" si="0"/>
-        <v>8.75</v>
-      </c>
-      <c r="I28" s="2">
-        <v>10</v>
-      </c>
-      <c r="J28" s="80">
-        <f>(I28/60)*G28</f>
         <v>8.75</v>
       </c>
     </row>
@@ -6505,14 +6507,14 @@
         <v>52.5</v>
       </c>
       <c r="H29" s="87">
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="I29" s="2">
+        <v>10</v>
+      </c>
+      <c r="J29" s="80">
         <f t="shared" si="0"/>
-        <v>8.75</v>
-      </c>
-      <c r="I29" s="2">
-        <v>10</v>
-      </c>
-      <c r="J29" s="80">
-        <f>(I29/60)*G29</f>
         <v>8.75</v>
       </c>
     </row>
@@ -6539,14 +6541,14 @@
         <v>52.5</v>
       </c>
       <c r="H30" s="87">
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+      <c r="I30" s="2">
+        <v>10</v>
+      </c>
+      <c r="J30" s="80">
         <f t="shared" si="0"/>
-        <v>8.75</v>
-      </c>
-      <c r="I30" s="2">
-        <v>10</v>
-      </c>
-      <c r="J30" s="80">
-        <f>(I30/60)*G30</f>
         <v>8.75</v>
       </c>
     </row>
@@ -6573,12 +6575,12 @@
         <v>52.5</v>
       </c>
       <c r="H31" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.125</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="80">
-        <f>(I31/60)*G31</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6605,12 +6607,12 @@
         <v>52.5</v>
       </c>
       <c r="H32" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.125</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="80">
-        <f>(I32/60)*G32</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6637,12 +6639,12 @@
         <v>52.5</v>
       </c>
       <c r="H33" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.125</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="80">
-        <f>(I33/60)*G33</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6669,12 +6671,12 @@
         <v>75</v>
       </c>
       <c r="H34" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>75</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="80">
-        <f>(I34/60)*G34</f>
+        <f t="shared" ref="J34:J65" si="2">(I34/60)*G34</f>
         <v>0</v>
       </c>
     </row>
@@ -6701,12 +6703,12 @@
         <v>75</v>
       </c>
       <c r="H35" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37.5</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="80">
-        <f>(I35/60)*G35</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -6733,12 +6735,12 @@
         <v>75</v>
       </c>
       <c r="H36" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37.5</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="80">
-        <f>(I36/60)*G36</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -6765,12 +6767,12 @@
         <v>75</v>
       </c>
       <c r="H37" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37.5</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="80">
-        <f>(I37/60)*G37</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -6797,14 +6799,14 @@
         <v>52.5</v>
       </c>
       <c r="H38" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.5</v>
       </c>
       <c r="I38" s="2">
         <v>10</v>
       </c>
       <c r="J38" s="80">
-        <f>(I38/60)*G38</f>
+        <f t="shared" si="2"/>
         <v>8.75</v>
       </c>
     </row>
@@ -6831,14 +6833,14 @@
         <v>52.5</v>
       </c>
       <c r="H39" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.5</v>
       </c>
       <c r="I39" s="2">
         <v>10</v>
       </c>
       <c r="J39" s="80">
-        <f>(I39/60)*G39</f>
+        <f t="shared" si="2"/>
         <v>8.75</v>
       </c>
     </row>
@@ -6865,14 +6867,14 @@
         <v>52.5</v>
       </c>
       <c r="H40" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52.5</v>
       </c>
       <c r="I40" s="2">
         <v>30</v>
       </c>
       <c r="J40" s="80">
-        <f>(I40/60)*G40</f>
+        <f t="shared" si="2"/>
         <v>26.25</v>
       </c>
     </row>
@@ -6899,12 +6901,12 @@
         <v>52.5</v>
       </c>
       <c r="H41" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52.5</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="80">
-        <f>(I41/60)*G41</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -6931,12 +6933,12 @@
         <v>52.5</v>
       </c>
       <c r="H42" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.125</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="80">
-        <f>(I42/60)*G42</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -6963,12 +6965,12 @@
         <v>52.5</v>
       </c>
       <c r="H43" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.5</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="80">
-        <f>(I43/60)*G43</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -6995,12 +6997,12 @@
         <v>52.5</v>
       </c>
       <c r="H44" s="90">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.5</v>
       </c>
       <c r="I44" s="20"/>
       <c r="J44" s="91">
-        <f>(I44/60)*G44</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -7027,14 +7029,14 @@
         <v>52.5</v>
       </c>
       <c r="H45" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
       <c r="I45" s="2">
         <v>5</v>
       </c>
       <c r="J45" s="80">
-        <f>(I45/60)*G45</f>
+        <f t="shared" si="2"/>
         <v>4.375</v>
       </c>
     </row>
@@ -7061,14 +7063,14 @@
         <v>52.5</v>
       </c>
       <c r="H46" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
       <c r="I46" s="2">
         <v>5</v>
       </c>
       <c r="J46" s="80">
-        <f>(I46/60)*G46</f>
+        <f t="shared" si="2"/>
         <v>4.375</v>
       </c>
     </row>
@@ -7095,14 +7097,14 @@
         <v>52.5</v>
       </c>
       <c r="H47" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
       <c r="I47" s="2">
         <v>5</v>
       </c>
       <c r="J47" s="80">
-        <f>(I47/60)*G47</f>
+        <f t="shared" si="2"/>
         <v>4.375</v>
       </c>
     </row>
@@ -7129,12 +7131,12 @@
         <v>52.5</v>
       </c>
       <c r="H48" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.125</v>
       </c>
       <c r="I48" s="68"/>
       <c r="J48" s="80">
-        <f>(I48/60)*G48</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -7161,12 +7163,12 @@
         <v>52.5</v>
       </c>
       <c r="H49" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="80">
-        <f>(I49/60)*G49</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -7193,12 +7195,12 @@
         <v>52.5</v>
       </c>
       <c r="H50" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="80">
-        <f>(I50/60)*G50</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -7225,12 +7227,12 @@
         <v>52.5</v>
       </c>
       <c r="H51" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="80">
-        <f>(I51/60)*G51</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -7257,14 +7259,14 @@
         <v>52.5</v>
       </c>
       <c r="H52" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
       <c r="I52" s="2">
         <v>5</v>
       </c>
       <c r="J52" s="80">
-        <f>(I52/60)*G52</f>
+        <f t="shared" si="2"/>
         <v>4.375</v>
       </c>
     </row>
@@ -7291,14 +7293,14 @@
         <v>52.5</v>
       </c>
       <c r="H53" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.125</v>
       </c>
       <c r="I53" s="2">
         <v>15</v>
       </c>
       <c r="J53" s="80">
-        <f>(I53/60)*G53</f>
+        <f t="shared" si="2"/>
         <v>13.125</v>
       </c>
     </row>
@@ -7325,14 +7327,14 @@
         <v>52.5</v>
       </c>
       <c r="H54" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
       <c r="I54" s="2">
         <v>10</v>
       </c>
       <c r="J54" s="80">
-        <f>(I54/60)*G54</f>
+        <f t="shared" si="2"/>
         <v>8.75</v>
       </c>
     </row>
@@ -7359,14 +7361,14 @@
         <v>52.5</v>
       </c>
       <c r="H55" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
       <c r="I55" s="2">
         <v>10</v>
       </c>
       <c r="J55" s="80">
-        <f>(I55/60)*G55</f>
+        <f t="shared" si="2"/>
         <v>8.75</v>
       </c>
     </row>
@@ -7393,14 +7395,14 @@
         <v>52.5</v>
       </c>
       <c r="H56" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
       <c r="I56" s="2">
         <v>10</v>
       </c>
       <c r="J56" s="80">
-        <f>(I56/60)*G56</f>
+        <f t="shared" si="2"/>
         <v>8.75</v>
       </c>
     </row>
@@ -7427,14 +7429,14 @@
         <v>52.5</v>
       </c>
       <c r="H57" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
       <c r="I57" s="2">
         <v>10</v>
       </c>
       <c r="J57" s="80">
-        <f>(I57/60)*G57</f>
+        <f t="shared" si="2"/>
         <v>8.75</v>
       </c>
     </row>
@@ -7461,14 +7463,14 @@
         <v>52.5</v>
       </c>
       <c r="H58" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
       <c r="I58" s="2">
         <v>10</v>
       </c>
       <c r="J58" s="80">
-        <f>(I58/60)*G58</f>
+        <f t="shared" si="2"/>
         <v>8.75</v>
       </c>
     </row>
@@ -7495,14 +7497,14 @@
         <v>52.5</v>
       </c>
       <c r="H59" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
       <c r="I59" s="2">
         <v>10</v>
       </c>
       <c r="J59" s="80">
-        <f>(I59/60)*G59</f>
+        <f t="shared" si="2"/>
         <v>8.75</v>
       </c>
     </row>
@@ -7529,14 +7531,14 @@
         <v>52.5</v>
       </c>
       <c r="H60" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
       <c r="I60" s="2">
         <v>10</v>
       </c>
       <c r="J60" s="80">
-        <f>(I60/60)*G60</f>
+        <f t="shared" si="2"/>
         <v>8.75</v>
       </c>
     </row>
@@ -7563,14 +7565,14 @@
         <v>52.5</v>
       </c>
       <c r="H61" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
       <c r="I61" s="2">
         <v>10</v>
       </c>
       <c r="J61" s="80">
-        <f>(I61/60)*G61</f>
+        <f t="shared" si="2"/>
         <v>8.75</v>
       </c>
     </row>
@@ -7597,14 +7599,14 @@
         <v>52.5</v>
       </c>
       <c r="H62" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
       <c r="I62" s="2">
         <v>10</v>
       </c>
       <c r="J62" s="80">
-        <f>(I62/60)*G62</f>
+        <f t="shared" si="2"/>
         <v>8.75</v>
       </c>
     </row>
@@ -7631,14 +7633,14 @@
         <v>52.5</v>
       </c>
       <c r="H63" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
       <c r="I63" s="2">
         <v>10</v>
       </c>
       <c r="J63" s="80">
-        <f>(I63/60)*G63</f>
+        <f t="shared" si="2"/>
         <v>8.75</v>
       </c>
     </row>
@@ -7665,14 +7667,14 @@
         <v>52.5</v>
       </c>
       <c r="H64" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
       <c r="I64" s="2">
         <v>10</v>
       </c>
       <c r="J64" s="80">
-        <f>(I64/60)*G64</f>
+        <f t="shared" si="2"/>
         <v>8.75</v>
       </c>
     </row>
@@ -7699,14 +7701,14 @@
         <v>52.5</v>
       </c>
       <c r="H65" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
       <c r="I65" s="2">
         <v>10</v>
       </c>
       <c r="J65" s="80">
-        <f>(I65/60)*G65</f>
+        <f t="shared" si="2"/>
         <v>8.75</v>
       </c>
     </row>
@@ -7733,14 +7735,14 @@
         <v>52.5</v>
       </c>
       <c r="H66" s="87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
       <c r="I66" s="2">
         <v>10</v>
       </c>
       <c r="J66" s="80">
-        <f>(I66/60)*G66</f>
+        <f t="shared" ref="J66:J97" si="3">(I66/60)*G66</f>
         <v>8.75</v>
       </c>
     </row>
@@ -7767,14 +7769,14 @@
         <v>52.5</v>
       </c>
       <c r="H67" s="87">
-        <f t="shared" ref="H67:H72" si="1">(E67/60)*G67</f>
+        <f t="shared" ref="H67:H72" si="4">(E67/60)*G67</f>
         <v>8.75</v>
       </c>
       <c r="I67" s="2">
         <v>10</v>
       </c>
       <c r="J67" s="80">
-        <f>(I67/60)*G67</f>
+        <f t="shared" si="3"/>
         <v>8.75</v>
       </c>
     </row>
@@ -7801,14 +7803,14 @@
         <v>75</v>
       </c>
       <c r="H68" s="87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>37.5</v>
       </c>
       <c r="I68" s="2">
         <v>10</v>
       </c>
       <c r="J68" s="80">
-        <f>(I68/60)*G68</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
     </row>
@@ -7842,7 +7844,7 @@
         <v>10</v>
       </c>
       <c r="J69" s="80">
-        <f>(I69/60)*G69</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
     </row>
@@ -7874,7 +7876,7 @@
         <v>300</v>
       </c>
       <c r="J70" s="110">
-        <f>(I70/60)*G70</f>
+        <f t="shared" si="3"/>
         <v>375</v>
       </c>
     </row>
@@ -7906,7 +7908,7 @@
         <v>200</v>
       </c>
       <c r="J71" s="110">
-        <f>(I71/60)*G71</f>
+        <f t="shared" si="3"/>
         <v>250</v>
       </c>
     </row>
@@ -7933,14 +7935,14 @@
         <v>52.5</v>
       </c>
       <c r="H72" s="108">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>420</v>
       </c>
       <c r="I72" s="109">
         <v>120</v>
       </c>
       <c r="J72" s="110">
-        <f>(I72/60)*G72</f>
+        <f t="shared" si="3"/>
         <v>105</v>
       </c>
     </row>

</xml_diff>